<commit_message>
perbaikan calculate days lagi
</commit_message>
<xml_diff>
--- a/results/summary.xlsx
+++ b/results/summary.xlsx
@@ -18,10 +18,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -60,12 +57,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -479,101 +475,101 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RSUD dr. R. GOETENG TAROENADIBRATA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
+          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RS HARAPAN IBU, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -583,16 +579,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
         <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>21</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -608,13 +604,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -623,48 +619,48 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RSUD AJIBARANG, KAB. BANYUMAS</t>
+          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
+          <t>RS ANANDA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -673,23 +669,23 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RS ISLAM PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -698,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -714,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -723,23 +719,23 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
@@ -748,13 +744,13 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RS AMANAH SUMPIUH, KAB. BANYUMAS</t>
+          <t>RS JIH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -764,157 +760,157 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RSUD dr. R. GOETENG TAROENADIBRATA, KAB. PURBALINGGA</t>
+          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS DADI KELUARGA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
+          <t>RS NIRMALA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
         <v>3</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>RS ANANDA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -923,23 +919,23 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RS JIH PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -948,98 +944,98 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ST. ELISABETH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
         <v>3</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RS DADI KELUARGA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RSUD AJIBARANG, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>RS NIRMALA, KAB. PURBALINGGA</t>
+          <t>RS ISLAM PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1048,24 +1044,24 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS HARAPAN IBU, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
         <v>4</v>
       </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>8</v>
-      </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
@@ -1073,23 +1069,23 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>RS ST. ELISABETH PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS AMANAH SUMPIUH, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1098,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1133,22 +1129,22 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="C28" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D28" t="n">
-        <v>206</v>
+        <v>240</v>
       </c>
       <c r="E28" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>352</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1158,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1200,178 +1196,178 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
+          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
         <v>3</v>
       </c>
-      <c r="D5" t="n">
-        <v>4</v>
-      </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RSUD AJIBARANG, KAB. BANYUMAS</t>
+          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>RS ISLAM PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RS AMANAH SUMPIUH, KAB. BANYUMAS</t>
+          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1381,102 +1377,102 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS DADI KELUARGA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
+          <t>RS ST. ELISABETH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
         <v>4</v>
@@ -1485,30 +1481,30 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>RS HARAPAN IBU, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS NIRMALA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>1</v>
@@ -1517,17 +1513,17 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RS DADI KELUARGA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RSUD AJIBARANG, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -1536,13 +1532,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS ISLAM PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1552,16 +1548,16 @@
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>RS NIRMALA, KAB. PURBALINGGA</t>
+          <t>RS AMANAH SUMPIUH, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1571,10 +1567,10 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1599,39 +1595,20 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PBG, KAB. PURBALINGGA</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>30</v>
-      </c>
-      <c r="C24" t="n">
-        <v>68</v>
-      </c>
-      <c r="D24" t="n">
-        <v>49</v>
-      </c>
-      <c r="E24" t="n">
-        <v>147</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C148"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1673,123 +1650,127 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>20-11-2024</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>45629</v>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>29-11-2024</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>45629</v>
+          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>22-11-2024</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RSUD AJIBARANG, KAB. BANYUMAS</t>
+          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>16-11-2024</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>18-11-2024</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16-11-2024</t>
+          <t>18-11-2024</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1804,466 +1785,466 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>30-11-2024</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RS ISLAM PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>21-11-2024</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>13-11-2024</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RS ISLAM PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>19-11-2024</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16-11-2024</t>
+          <t>23-11-2024</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>25-11-2024</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RS AMANAH SUMPIUH, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>30-11-2024</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>RS ISLAM PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS DADI KELUARGA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>02-12-2024</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ST. ELISABETH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>28-10-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>02-12-2024</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>02-12-2024</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>28-10-2024</t>
+          <t>20-11-2024</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>29-10-2024</t>
+          <t>23-11-2024</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>22-11-2024</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>20-11-2024</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>02-12-2024</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>05-11-2024</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>02-12-2024</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>22-11-2024</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>31-10-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS DADI KELUARGA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>25-11-2024</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -2274,17 +2255,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>23-11-2024</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2299,271 +2280,271 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>RS HARAPAN IBU, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>18-11-2024</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>02-12-2024</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>15-11-2024</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>21-11-2024</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>18-11-2024</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>RS DADI KELUARGA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>16-11-2024</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS NIRMALA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>20-11-2024</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62">
@@ -2574,17 +2555,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2599,217 +2580,217 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>18-11-2024</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>23-11-2024</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>16-11-2024</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>21-11-2024</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16-11-2024</t>
+          <t>22-11-2024</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>12-11-2024</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
+          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>21-11-2024</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>16-11-2024</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>RS HARAPAN IBU, KAB. PURBALINGGA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>RS HARAPAN IBU, KAB. PURBALINGGA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>14-11-2024</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2824,91 +2805,91 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>14-11-2024</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>16-11-2024</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>RS DADI KELUARGA PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>25-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>05-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85">
@@ -2919,56 +2900,56 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>25-11-2024</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>22-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>29-11-2024</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89">
@@ -2979,47 +2960,47 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RSUD AJIBARANG, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>23-11-2024</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3034,22 +3015,22 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>RS HARAPAN IBU, KAB. PURBALINGGA</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>16-11-2024</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3064,217 +3045,217 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>22-11-2024</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>25-11-2024</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>26-11-2024</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
+          <t>RS ISLAM PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>21-11-2024</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>15-11-2024</t>
+          <t>22-11-2024</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>14-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>22-11-2024</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS AMANAH SUMPIUH, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>22-11-2024</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>28-11-2024</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>16-11-2024</t>
+          <t>20-11-2024</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3289,586 +3270,106 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>RS NIRMALA, KAB. PURBALINGGA</t>
+          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>20-11-2024</t>
+          <t>16-11-2024</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS ANANDA PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>02-11-2024</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
+          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>20-04-2024</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>14</v>
+        <v>227</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
+          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>19-11-2024</t>
+          <t>22-04-2024</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>14</v>
+        <v>225</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
+          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>21-11-2024</t>
+          <t>17-09-2024</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
+          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>18-11-2024</t>
+          <t>05-08-2024</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>15</v>
+        <v>120</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>RS PKU MUHAMMADIYAH BANJARNEGARA, KAB. BANJARNEGARA</t>
+          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>23-11-2024</t>
+          <t>01-08-2024</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>16-11-2024</t>
-        </is>
-      </c>
-      <c r="C117" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>RS HARAPAN IBU, KAB. PURBALINGGA</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>21-11-2024</t>
-        </is>
-      </c>
-      <c r="C118" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>RS TK.III WIJAYAKUSUMA PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>21-11-2024</t>
-        </is>
-      </c>
-      <c r="C119" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>RS MEDIKA LESTARI, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>12-11-2024</t>
-        </is>
-      </c>
-      <c r="C120" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>21-11-2024</t>
-        </is>
-      </c>
-      <c r="C121" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>19-11-2024</t>
-        </is>
-      </c>
-      <c r="C122" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>16-11-2024</t>
-        </is>
-      </c>
-      <c r="C123" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>14-11-2024</t>
-        </is>
-      </c>
-      <c r="C124" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>14-11-2024</t>
-        </is>
-      </c>
-      <c r="C125" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>RS SIAGA MEDIKA PURBALINGGA, KAB. PURBALINGGA</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>14-11-2024</t>
-        </is>
-      </c>
-      <c r="C126" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>16-11-2024</t>
-        </is>
-      </c>
-      <c r="C127" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>16-11-2024</t>
-        </is>
-      </c>
-      <c r="C128" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>16-11-2024</t>
-        </is>
-      </c>
-      <c r="C129" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>RS ANANDA PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>02-11-2024</t>
-        </is>
-      </c>
-      <c r="C130" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>12-09-2024</t>
-        </is>
-      </c>
-      <c r="C131" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>RS ORTHOPAEDI PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>12-09-2024</t>
-        </is>
-      </c>
-      <c r="C132" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>20-04-2024</t>
-        </is>
-      </c>
-      <c r="C133" t="n">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>22-04-2024</t>
-        </is>
-      </c>
-      <c r="C134" t="n">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>RS EMANUEL BANJARNEGARA, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>17-09-2024</t>
-        </is>
-      </c>
-      <c r="C135" t="n">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>21-08-2024</t>
-        </is>
-      </c>
-      <c r="C136" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>21-08-2024</t>
-        </is>
-      </c>
-      <c r="C137" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>RS SIAGA MEDIKA BANYUMAS, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>21-08-2024</t>
-        </is>
-      </c>
-      <c r="C138" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>21-08-2024</t>
-        </is>
-      </c>
-      <c r="C139" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>21-08-2024</t>
-        </is>
-      </c>
-      <c r="C140" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>RS WIRADADI HUSADA, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>05-08-2024</t>
-        </is>
-      </c>
-      <c r="C141" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>RSUD HJ ANNA LASMANAH, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>12-08-2024</t>
-        </is>
-      </c>
-      <c r="C142" t="n">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>RS ISLAM AT-TIN HUSADA, KAB. PURBALINGGA</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>10-08-2024</t>
-        </is>
-      </c>
-      <c r="C143" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>RS ISLAM BANJARNEGARA, KAB. BANJARNEGARA</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>01-08-2024</t>
-        </is>
-      </c>
-      <c r="C144" t="n">
         <v>124</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>RSUD MARGONO SOEKARJO PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>02-07-2024</t>
-        </is>
-      </c>
-      <c r="C145" t="n">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>RS NIRMALA, KAB. PURBALINGGA</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>01-07-2024</t>
-        </is>
-      </c>
-      <c r="C146" t="n">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>RS SINAR KASIH PURWOKERTO, KAB. BANYUMAS</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>24-06-2024</t>
-        </is>
-      </c>
-      <c r="C147" t="n">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>RS SIAGA MEDIKA PBG, KAB. PURBALINGGA</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>17-05-2024</t>
-        </is>
-      </c>
-      <c r="C148" t="n">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>